<commit_message>
Added scripts and spreadsheet to concurrent sum
</commit_message>
<xml_diff>
--- a/testes/MM/J5_Log_excel.xlsx
+++ b/testes/MM/J5_Log_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACEW\Documents\Android\androidconcurrency\testes\MM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0F78C5B8-98A5-4868-8693-00F60532E521}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5CD916A6-8C13-4D37-A232-3640332E740A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
@@ -1088,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added firebase test to MM
</commit_message>
<xml_diff>
--- a/testes/MM/J5_Log_excel.xlsx
+++ b/testes/MM/J5_Log_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACEW\Documents\Android\androidconcurrency\testes\MM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07F1422-B733-46E6-A243-1CD8AC1CC4B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72838D22-7F8F-4733-AA5E-967594335BF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10080" yWindow="3135" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="J5_Log_agreggated" sheetId="1" r:id="rId1"/>
@@ -4874,16 +4874,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>214993</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>106136</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>484909</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>175409</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>952501</xdr:colOff>
-      <xdr:row>107</xdr:row>
-      <xdr:rowOff>54429</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>813956</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>123702</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5212,8 +5212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AJ95" sqref="AJ95"/>
+    <sheetView tabSelected="1" topLeftCell="AC73" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AF34" sqref="AF34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>